<commit_message>
Ill try harder next time, I promise
</commit_message>
<xml_diff>
--- a/Challenges/Semester 2 Week 11 - Build and Query Challenge Resit 2/Build_Query_Challenge_Caterer_SAMPLE_DATA.xlsx
+++ b/Challenges/Semester 2 Week 11 - Build and Query Challenge Resit 2/Build_Query_Challenge_Caterer_SAMPLE_DATA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://liveswinburneeduau-my.sharepoint.com/personal/tbaird_swin_edu_au/Documents/Swinburne/Teaching/2021/semester 2/DAD/Assessments/Build Query Challenge/Resit Challenge 2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://liveswinburneeduau-my.sharepoint.com/personal/103577332_student_swin_edu_au/Documents/Cert IV IT 2021/Databases/Challenges/Semester 2 Week 11 - Build and Query Challenge Resit 2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="193" documentId="8_{423D5E0E-9EE2-E846-92C4-7F99EB6B5AF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DE20C7CF-3912-1B47-AEAF-CC902645C15A}"/>
+  <xr:revisionPtr revIDLastSave="198" documentId="8_{423D5E0E-9EE2-E846-92C4-7F99EB6B5AF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{86BE1560-BAFD-4321-8C48-99520DA15E9A}"/>
   <bookViews>
-    <workbookView xWindow="400" yWindow="680" windowWidth="22980" windowHeight="16940" xr2:uid="{F298CE2B-884A-2C4F-9CA7-FF48B922ED27}"/>
+    <workbookView xWindow="28875" yWindow="45" windowWidth="10575" windowHeight="15645" xr2:uid="{F298CE2B-884A-2C4F-9CA7-FF48B922ED27}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="42">
   <si>
     <t>Organisation</t>
   </si>
@@ -51,9 +51,6 @@
     <t>Swinburne University of Technology</t>
   </si>
   <si>
-    <t>Client ID</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
@@ -157,6 +154,12 @@
   </si>
   <si>
     <t>The George - 1 John Street, Hawthorn, 3122</t>
+  </si>
+  <si>
+    <t>Ibrahim Oztas</t>
+  </si>
+  <si>
+    <t>(03)5555-4569</t>
   </si>
 </sst>
 </file>
@@ -164,8 +167,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="d/mm/yyyy;@"/>
+    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="d/mm/yyyy;@"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -221,7 +224,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -231,13 +234,13 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -560,18 +563,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72A1ECB3-C8C4-2140-9397-42A66A4E03C0}">
   <dimension ref="A1:G48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="32" customWidth="1"/>
-    <col min="3" max="3" width="47.33203125" customWidth="1"/>
-    <col min="4" max="4" width="22.6640625" customWidth="1"/>
+    <col min="3" max="3" width="47.296875" customWidth="1"/>
+    <col min="4" max="4" width="22.69921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -582,7 +585,7 @@
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -595,12 +598,12 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>11</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -608,7 +611,7 @@
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -621,7 +624,7 @@
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -630,7 +633,7 @@
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -639,9 +642,9 @@
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
@@ -650,15 +653,15 @@
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="C8" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>7</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>1</v>
@@ -667,15 +670,15 @@
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>12</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>3</v>
@@ -684,32 +687,32 @@
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>15</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="D10" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>18</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>3</v>
@@ -718,33 +721,41 @@
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>21</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>23</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -753,9 +764,9 @@
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
@@ -764,26 +775,26 @@
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="C16" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="D16" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>3214</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C17" s="1">
         <v>2</v>
@@ -792,12 +803,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>3216</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C18" s="1">
         <v>1</v>
@@ -806,12 +817,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>3218</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C19" s="1">
         <v>4</v>
@@ -820,12 +831,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>4325</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C20" s="1">
         <v>1</v>
@@ -834,12 +845,12 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>4326</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C21" s="1">
         <v>1</v>
@@ -848,12 +859,12 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>4327</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C22" s="1">
         <v>1</v>
@@ -862,25 +873,25 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B26" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>12</v>
       </c>
@@ -888,10 +899,10 @@
         <v>44459</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>21</v>
       </c>
@@ -899,10 +910,10 @@
         <v>44453</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>21</v>
       </c>
@@ -910,10 +921,10 @@
         <v>44466</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>15</v>
       </c>
@@ -921,10 +932,10 @@
         <v>44459</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>18</v>
       </c>
@@ -932,32 +943,32 @@
         <v>44469</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B34" s="6"/>
       <c r="C34" s="6"/>
       <c r="D34" s="6"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B35" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="C35" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D35" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C35" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>3216</v>
       </c>
@@ -971,7 +982,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>4326</v>
       </c>
@@ -985,7 +996,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>3218</v>
       </c>
@@ -999,7 +1010,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>3214</v>
       </c>
@@ -1013,7 +1024,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>4325</v>
       </c>
@@ -1027,7 +1038,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>4327</v>
       </c>
@@ -1041,7 +1052,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>3216</v>
       </c>
@@ -1055,7 +1066,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>4327</v>
       </c>
@@ -1069,7 +1080,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>3218</v>
       </c>
@@ -1083,7 +1094,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>3216</v>
       </c>
@@ -1097,7 +1108,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>4326</v>
       </c>
@@ -1111,7 +1122,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>3216</v>
       </c>
@@ -1125,7 +1136,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>4327</v>
       </c>

</xml_diff>